<commit_message>
upd to board 1.2
should fix transistor footprint and shift diodes
</commit_message>
<xml_diff>
--- a/BOM.Guide.xlsx
+++ b/BOM.Guide.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="198">
   <si>
     <t>Source:</t>
   </si>
@@ -598,7 +598,31 @@
     <t>incoming eBay 2022</t>
   </si>
   <si>
-    <t>OPA4171 or maybe TL074 IDK</t>
+    <t>R24, R26, R27, R29</t>
+  </si>
+  <si>
+    <t>PJ301 THONKICONN6</t>
+  </si>
+  <si>
+    <t>OPA4171</t>
+  </si>
+  <si>
+    <t>a tl074 almost works but the fancy opamp is better</t>
+  </si>
+  <si>
+    <t>J112 works too. Trying others.</t>
+  </si>
+  <si>
+    <t>pre-bend to lay flat on board inside</t>
+  </si>
+  <si>
+    <t>Capacitor_THT:D6.3mm_P2.50mm</t>
+  </si>
+  <si>
+    <t>R27 sets noise volume</t>
+  </si>
+  <si>
+    <t>output protections, could be 100R to 1K</t>
   </si>
 </sst>
 </file>
@@ -2774,10 +2798,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2825,7 +2849,9 @@
       <c r="E2" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="5" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
@@ -2904,10 +2930,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>136</v>
@@ -2915,7 +2941,9 @@
       <c r="E7" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
@@ -2925,10 +2953,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>166</v>
@@ -2943,10 +2971,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>166</v>
@@ -2961,55 +2989,57 @@
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>145</v>
+        <v>22</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>146</v>
+        <v>23</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F10" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>22</v>
+        <v>171</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>171</v>
+        <v>34</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="F12" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -3017,36 +3047,36 @@
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>39</v>
+        <v>153</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>165</v>
+        <v>48</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -3054,22 +3084,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>153</v>
+        <v>66</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -3077,10 +3107,10 @@
         <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>189</v>
+        <v>58</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>61</v>
@@ -3095,13 +3125,13 @@
         <v>1</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F17" s="5"/>
     </row>
@@ -3113,34 +3143,36 @@
         <v>1</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="5"/>
+        <v>185</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>98</v>
+        <v>158</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>185</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -3148,19 +3180,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>158</v>
+        <v>94</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -3177,9 +3209,11 @@
         <v>18</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="5"/>
+        <v>195</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
@@ -3237,43 +3271,23 @@
       </c>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>95</v>
+        <v>155</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>190</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
-        <v>25</v>
-      </c>
-      <c r="B26" s="3">
-        <v>12</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="F26" s="5"/>
+      <c r="F25" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
update for noise level
</commit_message>
<xml_diff>
--- a/BOM.Guide.xlsx
+++ b/BOM.Guide.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="500" windowWidth="19120" windowHeight="17500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="6240" yWindow="500" windowWidth="19120" windowHeight="17500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
     <sheet name="GUIDE" sheetId="2" r:id="rId2"/>
     <sheet name="Costing" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -595,9 +595,6 @@
     <t>incoming eBay 2022</t>
   </si>
   <si>
-    <t>R24, R26, R27, R29</t>
-  </si>
-  <si>
     <t>PJ301 THONKICONN6</t>
   </si>
   <si>
@@ -607,9 +604,6 @@
     <t>a tl074 almost works but the fancy opamp is better</t>
   </si>
   <si>
-    <t>J112 works too. Trying others.</t>
-  </si>
-  <si>
     <t>pre-bend to lay flat on board inside</t>
   </si>
   <si>
@@ -659,6 +653,12 @@
   </si>
   <si>
     <t>Total Kit Price estimate</t>
+  </si>
+  <si>
+    <t>R27, R30</t>
+  </si>
+  <si>
+    <t>J112 and MMBF4392 work too</t>
   </si>
 </sst>
 </file>
@@ -2870,8 +2870,8 @@
   </sheetPr>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2885,7 +2885,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2925,7 +2925,7 @@
         <v>166</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -3005,19 +3005,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>136</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>166</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -3025,10 +3022,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>143</v>
+        <v>208</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>144</v>
@@ -3036,7 +3033,9 @@
       <c r="E9" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
@@ -3165,13 +3164,13 @@
         <v>66</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>190</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -3188,7 +3187,7 @@
         <v>59</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F17" s="5"/>
     </row>
@@ -3206,7 +3205,7 @@
         <v>63</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F18" s="5"/>
     </row>
@@ -3227,7 +3226,7 @@
         <v>185</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>192</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -3267,7 +3266,7 @@
         <v>174</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -3284,10 +3283,10 @@
         <v>18</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -3357,7 +3356,7 @@
         <v>155</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>184</v>
@@ -3401,13 +3400,13 @@
         <v>169</v>
       </c>
       <c r="G1" t="s">
+        <v>201</v>
+      </c>
+      <c r="H1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I1" t="s">
         <v>203</v>
-      </c>
-      <c r="H1" t="s">
-        <v>204</v>
-      </c>
-      <c r="I1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="48" x14ac:dyDescent="0.2">
@@ -3463,13 +3462,13 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K3" t="s">
+        <v>204</v>
+      </c>
+      <c r="L3" t="s">
         <v>206</v>
       </c>
-      <c r="L3" t="s">
-        <v>208</v>
-      </c>
       <c r="M3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="48" x14ac:dyDescent="0.2">
@@ -3602,7 +3601,7 @@
         <v>166</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H8" s="13">
         <v>0.01</v>
@@ -4093,7 +4092,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H27" s="13">
         <v>1</v>
@@ -4105,7 +4104,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C28" s="9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>